<commit_message>
Updates to customer data
</commit_message>
<xml_diff>
--- a/CustomerData.xlsx
+++ b/CustomerData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>CustomerId</t>
   </si>
@@ -37,6 +37,42 @@
   </si>
   <si>
     <t>fdgdsfgd</t>
+  </si>
+  <si>
+    <t>Field of Purchase</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>Cloths</t>
+  </si>
+  <si>
+    <t>sports</t>
+  </si>
+  <si>
+    <t>Delicacies</t>
+  </si>
+  <si>
+    <t>OTT</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>china</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Mexico</t>
   </si>
 </sst>
 </file>
@@ -368,60 +404,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>200</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>300</v>
       </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>400</v>
       </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>1000</v>
       </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>20000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>